<commit_message>
updated ramp cards to decklist
</commit_message>
<xml_diff>
--- a/MTG/EDHDeckList.xlsx
+++ b/MTG/EDHDeckList.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="360" yWindow="105" windowWidth="13395" windowHeight="7740"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="DeckList" sheetId="1" r:id="rId1"/>
+    <sheet name="ManaGrid" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="106">
   <si>
     <t>Kabira Crossroads</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Windbrisk Heights</t>
   </si>
   <si>
-    <t>Copy and Paste</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -150,7 +147,193 @@
     <t>Pearl Medallion</t>
   </si>
   <si>
+    <t>Enchantment</t>
+  </si>
+  <si>
     <t>Synergy</t>
+  </si>
+  <si>
+    <t>BuyList</t>
+  </si>
+  <si>
+    <t>Knight of the White Orchid</t>
+  </si>
+  <si>
+    <t>Weathered Wayfarer</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Ramp</t>
+  </si>
+  <si>
+    <t>Wall</t>
+  </si>
+  <si>
+    <t>Overgrown Battlement</t>
+  </si>
+  <si>
+    <t>MazeEnd</t>
+  </si>
+  <si>
+    <t>MaikoTsunami</t>
+  </si>
+  <si>
+    <t>Nature's Lore</t>
+  </si>
+  <si>
+    <t>Cultivate</t>
+  </si>
+  <si>
+    <t>Kodama's Reach</t>
+  </si>
+  <si>
+    <t>Explosive Vegetation</t>
+  </si>
+  <si>
+    <t>Explore</t>
+  </si>
+  <si>
+    <t>Urban Evolution</t>
+  </si>
+  <si>
+    <t>Lotus Cobra</t>
+  </si>
+  <si>
+    <t>Kalani Expedition</t>
+  </si>
+  <si>
+    <t>Exploration</t>
+  </si>
+  <si>
+    <t>Harmonize</t>
+  </si>
+  <si>
+    <t>Reap and Sow</t>
+  </si>
+  <si>
+    <t>Harrow</t>
+  </si>
+  <si>
+    <t>Rampant Growth</t>
+  </si>
+  <si>
+    <t>Summer Bloom</t>
+  </si>
+  <si>
+    <t>Land Tax</t>
+  </si>
+  <si>
+    <t>Dreamscape Artist</t>
+  </si>
+  <si>
+    <t>Bog Witch</t>
+  </si>
+  <si>
+    <t>Nekusar</t>
+  </si>
+  <si>
+    <t>Kami</t>
+  </si>
+  <si>
+    <t>Talrand</t>
+  </si>
+  <si>
+    <t>MonoGreenDevotion</t>
+  </si>
+  <si>
+    <t>Snake</t>
+  </si>
+  <si>
+    <t>Azusa, Lost But Seeking</t>
+  </si>
+  <si>
+    <t>Draw</t>
+  </si>
+  <si>
+    <t>Sorcery</t>
+  </si>
+  <si>
+    <t>Instant</t>
+  </si>
+  <si>
+    <t>Marshal's Anthem</t>
+  </si>
+  <si>
+    <t>Mentor of the Meek</t>
+  </si>
+  <si>
+    <t>Doran</t>
+  </si>
+  <si>
+    <t>Twincast</t>
+  </si>
+  <si>
+    <t>Hidden Strings</t>
+  </si>
+  <si>
+    <t>Dark Ritual</t>
+  </si>
+  <si>
+    <t>Recross the Paths</t>
+  </si>
+  <si>
+    <t>Boundless Realms</t>
+  </si>
+  <si>
+    <t>Bird's of Paradise</t>
+  </si>
+  <si>
+    <t>Clone</t>
+  </si>
+  <si>
+    <t>Mana Reflection</t>
+  </si>
+  <si>
+    <t>Path to Exile</t>
+  </si>
+  <si>
+    <t>Garruk Wildspeaker</t>
+  </si>
+  <si>
+    <t>Braid of Fire</t>
+  </si>
+  <si>
+    <t>Skyshroud Claim</t>
+  </si>
+  <si>
+    <t>Ranger's Path</t>
+  </si>
+  <si>
+    <t>Sylvan Caryatid</t>
+  </si>
+  <si>
+    <t>Somber Sage</t>
+  </si>
+  <si>
+    <t>Rofellos, Llanowar Emissary</t>
+  </si>
+  <si>
+    <t>Oracle of Mul Daya</t>
+  </si>
+  <si>
+    <t>Primal Growth</t>
+  </si>
+  <si>
+    <t>Utopia Tree</t>
+  </si>
+  <si>
+    <t>Sakura-Tribe Elder</t>
+  </si>
+  <si>
+    <t>Elvish Mystic</t>
+  </si>
+  <si>
+    <t>Voyaging Satyr</t>
+  </si>
+  <si>
+    <t>Market Festival</t>
   </si>
 </sst>
 </file>
@@ -197,11 +380,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,50 +701,50 @@
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -566,29 +752,29 @@
       <c r="F2" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G2" t="str">
-        <f>"1 "&amp;E2</f>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="str">
+        <f>IF(G2="Owned","","1 "&amp;E2)</f>
         <v>1 Daru Encampment</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -596,29 +782,29 @@
       <c r="F3" s="1">
         <v>0.05</v>
       </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G42" si="0">"1 "&amp;E3</f>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I45" si="0">IF(G3="Owned","","1 "&amp;E3)</f>
         <v>1 Drifting Meadow</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -626,29 +812,29 @@
       <c r="F4" s="1">
         <v>7.2</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="str">
         <f t="shared" si="0"/>
         <v>1 Eiganjo Castle</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -656,29 +842,29 @@
       <c r="F5" s="1">
         <v>1.99</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="str">
         <f t="shared" si="0"/>
         <v>1 Emeria, the Sky Ruin</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -686,29 +872,29 @@
       <c r="F6" s="1">
         <v>7.88</v>
       </c>
-      <c r="G6" t="str">
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="str">
         <f t="shared" si="0"/>
         <v>1 Flagstones of Trokair</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -716,29 +902,29 @@
       <c r="F7" s="1">
         <v>0.22</v>
       </c>
-      <c r="G7" t="str">
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="str">
         <f t="shared" si="0"/>
         <v>1 Forbidding Watch Tower</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
@@ -746,29 +932,29 @@
       <c r="F8" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G8" t="str">
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="str">
         <f t="shared" si="0"/>
         <v>1 Kabira Crossroads</v>
-      </c>
-      <c r="H8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -776,29 +962,29 @@
       <c r="F9" s="1">
         <v>0.05</v>
       </c>
-      <c r="G9" t="str">
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="str">
         <f t="shared" si="0"/>
         <v>1 Karoo</v>
-      </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -806,29 +992,29 @@
       <c r="F10" s="1">
         <v>2.79</v>
       </c>
-      <c r="G10" t="str">
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="str">
         <f t="shared" si="0"/>
         <v>1 Kjeldoran Outpost</v>
-      </c>
-      <c r="H10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -836,29 +1022,29 @@
       <c r="F11" s="1">
         <v>2.66</v>
       </c>
-      <c r="G11" t="str">
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" t="str">
         <f t="shared" si="0"/>
         <v>1 Mistveil Plains</v>
-      </c>
-      <c r="H11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -866,29 +1052,29 @@
       <c r="F12" s="1">
         <v>0.09</v>
       </c>
-      <c r="G12" t="str">
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" t="str">
         <f t="shared" si="0"/>
         <v>1 New Benalia</v>
-      </c>
-      <c r="H12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -896,29 +1082,29 @@
       <c r="F13" s="1">
         <v>0.05</v>
       </c>
-      <c r="G13" t="str">
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" t="str">
         <f t="shared" si="0"/>
         <v>1 Secluded Steppe</v>
-      </c>
-      <c r="H13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -926,29 +1112,29 @@
       <c r="F14" s="1">
         <v>0.09</v>
       </c>
-      <c r="G14" t="str">
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" t="str">
         <f t="shared" si="0"/>
         <v>1 Sejiri Steppe</v>
-      </c>
-      <c r="H14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -956,801 +1142,1488 @@
       <c r="F15" s="1">
         <v>0.45</v>
       </c>
-      <c r="G15" t="str">
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" t="str">
         <f t="shared" si="0"/>
         <v>1 Windbrisk Heights</v>
-      </c>
-      <c r="H15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G16" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G16" t="s">
+        <v>25</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G17" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G17" t="s">
+        <v>25</v>
       </c>
       <c r="H17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G18" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G18" t="s">
+        <v>25</v>
       </c>
       <c r="H18" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F19" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G19" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G19" t="s">
+        <v>25</v>
       </c>
       <c r="H19" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G20" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G20" t="s">
+        <v>25</v>
       </c>
       <c r="H20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G21" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G21" t="s">
+        <v>25</v>
       </c>
       <c r="H21" t="s">
-        <v>26</v>
-      </c>
-      <c r="I21" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F22" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G22" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G22" t="s">
+        <v>25</v>
       </c>
       <c r="H22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I22" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F23" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G23" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G23" t="s">
+        <v>25</v>
       </c>
       <c r="H23" t="s">
-        <v>26</v>
-      </c>
-      <c r="I23" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G24" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G24" t="s">
+        <v>25</v>
       </c>
       <c r="H24" t="s">
-        <v>26</v>
-      </c>
-      <c r="I24" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G25" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G25" t="s">
+        <v>25</v>
       </c>
       <c r="H25" t="s">
-        <v>26</v>
-      </c>
-      <c r="I25" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F26" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G26" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G26" t="s">
+        <v>25</v>
       </c>
       <c r="H26" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F27" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G27" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G27" t="s">
+        <v>25</v>
       </c>
       <c r="H27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I27" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F28" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G28" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G28" t="s">
+        <v>25</v>
       </c>
       <c r="H28" t="s">
-        <v>26</v>
-      </c>
-      <c r="I28" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F29" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G29" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G29" t="s">
+        <v>25</v>
       </c>
       <c r="H29" t="s">
-        <v>26</v>
-      </c>
-      <c r="I29" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F30" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G30" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G30" t="s">
+        <v>25</v>
       </c>
       <c r="H30" t="s">
-        <v>26</v>
-      </c>
-      <c r="I30" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G31" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G31" t="s">
+        <v>25</v>
       </c>
       <c r="H31" t="s">
-        <v>26</v>
-      </c>
-      <c r="I31" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F32" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G32" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G32" t="s">
+        <v>25</v>
       </c>
       <c r="H32" t="s">
-        <v>26</v>
-      </c>
-      <c r="I32" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F33" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G33" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G33" t="s">
+        <v>25</v>
       </c>
       <c r="H33" t="s">
-        <v>26</v>
-      </c>
-      <c r="I33" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F34" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G34" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G34" t="s">
+        <v>25</v>
       </c>
       <c r="H34" t="s">
-        <v>26</v>
-      </c>
-      <c r="I34" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F35" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G35" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G35" t="s">
+        <v>25</v>
       </c>
       <c r="H35" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F36" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G36" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G36" t="s">
+        <v>25</v>
       </c>
       <c r="H36" t="s">
-        <v>26</v>
-      </c>
-      <c r="I36" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F37" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G37" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Plains</v>
+      <c r="G37" t="s">
+        <v>25</v>
       </c>
       <c r="H37" t="s">
-        <v>26</v>
-      </c>
-      <c r="I37" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
         <v>36</v>
       </c>
-      <c r="C38" t="s">
-        <v>37</v>
-      </c>
       <c r="D38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F38" s="1">
         <v>0.1</v>
       </c>
-      <c r="G38" t="str">
+      <c r="H38" t="s">
+        <v>31</v>
+      </c>
+      <c r="I38" t="str">
         <f t="shared" si="0"/>
         <v>1 Dispeller's Capsule</v>
-      </c>
-      <c r="I38" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F39" s="1">
         <v>0.22</v>
       </c>
-      <c r="G39" t="str">
+      <c r="H39" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" t="str">
         <f t="shared" si="0"/>
         <v>1 Marble Diamond</v>
-      </c>
-      <c r="I39" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F40" s="1">
         <v>0.75</v>
       </c>
-      <c r="G40" t="str">
+      <c r="H40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" t="str">
         <f t="shared" si="0"/>
         <v>1 Norn's Annex</v>
-      </c>
-      <c r="I40" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
       </c>
-      <c r="G41" t="str">
-        <f t="shared" si="0"/>
-        <v>1 Spear of Heliod</v>
+      <c r="G41" t="s">
+        <v>25</v>
       </c>
       <c r="H41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I41" t="s">
         <v>44</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F42" s="1">
         <v>0.75</v>
       </c>
-      <c r="G42" t="str">
+      <c r="H42" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" t="str">
         <f t="shared" si="0"/>
         <v>1 Pearl Medallion</v>
       </c>
-      <c r="I42" t="s">
-        <v>31</v>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" t="s">
+        <v>46</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="0"/>
+        <v>1 Knight of the White Orchid</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="0"/>
+        <v>1 Weathered Wayfarer</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" t="s">
+        <v>51</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="0"/>
+        <v>1 Overgrown Battlement</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" t="s">
+        <v>78</v>
+      </c>
+      <c r="D51" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D53" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" t="s">
+        <v>43</v>
+      </c>
+      <c r="D55" t="s">
+        <v>49</v>
+      </c>
+      <c r="E55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56" t="s">
+        <v>49</v>
+      </c>
+      <c r="E56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" t="s">
+        <v>49</v>
+      </c>
+      <c r="E58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" t="s">
+        <v>43</v>
+      </c>
+      <c r="D59" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60" t="s">
+        <v>43</v>
+      </c>
+      <c r="D60" t="s">
+        <v>49</v>
+      </c>
+      <c r="E60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" t="s">
+        <v>77</v>
+      </c>
+      <c r="E61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" t="s">
+        <v>77</v>
+      </c>
+      <c r="E62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" t="s">
+        <v>49</v>
+      </c>
+      <c r="E64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D65" t="s">
+        <v>49</v>
+      </c>
+      <c r="E65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>74</v>
+      </c>
+      <c r="D66" t="s">
+        <v>49</v>
+      </c>
+      <c r="E66" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" t="s">
+        <v>43</v>
+      </c>
+      <c r="D67" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" t="s">
+        <v>48</v>
+      </c>
+      <c r="D68" t="s">
+        <v>49</v>
+      </c>
+      <c r="E68" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" t="s">
+        <v>36</v>
+      </c>
+      <c r="C69" t="s">
+        <v>48</v>
+      </c>
+      <c r="D69" t="s">
+        <v>49</v>
+      </c>
+      <c r="E69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" t="s">
+        <v>49</v>
+      </c>
+      <c r="E70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" t="s">
+        <v>41</v>
+      </c>
+      <c r="E71" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" t="s">
+        <v>77</v>
+      </c>
+      <c r="E72" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" t="s">
+        <v>77</v>
+      </c>
+      <c r="E73" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="D74" t="s">
+        <v>89</v>
+      </c>
+      <c r="E74" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>73</v>
+      </c>
+      <c r="D75" t="s">
+        <v>49</v>
+      </c>
+      <c r="E75" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>71</v>
+      </c>
+      <c r="D76" t="s">
+        <v>49</v>
+      </c>
+      <c r="E76" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>74</v>
+      </c>
+      <c r="D77" t="s">
+        <v>49</v>
+      </c>
+      <c r="E77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>74</v>
+      </c>
+      <c r="D78" t="s">
+        <v>49</v>
+      </c>
+      <c r="E78" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>53</v>
+      </c>
+      <c r="D79" t="s">
+        <v>49</v>
+      </c>
+      <c r="E79" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>53</v>
+      </c>
+      <c r="B80" t="s">
+        <v>43</v>
+      </c>
+      <c r="D80" t="s">
+        <v>49</v>
+      </c>
+      <c r="E80" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>74</v>
+      </c>
+      <c r="B81" t="s">
+        <v>43</v>
+      </c>
+      <c r="D81" t="s">
+        <v>49</v>
+      </c>
+      <c r="E81" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>18</v>
+      </c>
+      <c r="E82" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>74</v>
+      </c>
+      <c r="E83" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>71</v>
+      </c>
+      <c r="E84" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>74</v>
+      </c>
+      <c r="E85" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>74</v>
+      </c>
+      <c r="E86" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>53</v>
+      </c>
+      <c r="E87" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>53</v>
+      </c>
+      <c r="E88" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>74</v>
+      </c>
+      <c r="E89" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>53</v>
+      </c>
+      <c r="E90" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>74</v>
+      </c>
+      <c r="E91" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>74</v>
+      </c>
+      <c r="E92" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>53</v>
+      </c>
+      <c r="E93" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>74</v>
+      </c>
+      <c r="E94" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>53</v>
+      </c>
+      <c r="E95" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>74</v>
+      </c>
+      <c r="E96" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>53</v>
+      </c>
+      <c r="E97" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E98" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E99" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>